<commit_message>
Régénération du planning mai 2026
Planning mis à jour avec les nouvelles règles de répartition (1.09.2025)

https://claude.ai/code/session_013GVFUnsuJT5neVS5zgeUHQ
</commit_message>
<xml_diff>
--- a/sorties/05 - MAI 2026.xlsx
+++ b/sorties/05 - MAI 2026.xlsx
@@ -165,12 +165,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF9999"/>
-        <bgColor rgb="FFFF9999"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFCE4D6"/>
         <bgColor rgb="FFFCE4D6"/>
       </patternFill>
@@ -185,6 +179,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF9933"/>
         <bgColor rgb="FFFF9933"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9999"/>
+        <bgColor rgb="FFFF9999"/>
       </patternFill>
     </fill>
     <fill>
@@ -325,34 +325,34 @@
     <xf numFmtId="0" fontId="3" fillId="19" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="20" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="23" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -364,7 +364,7 @@
     <xf numFmtId="0" fontId="3" fillId="24" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -1634,7 +1634,7 @@
       <c r="L17" s="8" t="n"/>
       <c r="M17" s="8" t="n"/>
       <c r="N17" s="24" t="n"/>
-      <c r="O17" s="8" t="n"/>
+      <c r="O17" s="24" t="n"/>
       <c r="P17" s="8" t="n"/>
       <c r="Q17" s="24" t="n"/>
       <c r="R17" s="8" t="n"/>
@@ -1677,7 +1677,7 @@
       <c r="L18" s="8" t="n"/>
       <c r="M18" s="8" t="n"/>
       <c r="N18" s="10" t="n"/>
-      <c r="O18" s="26" t="n"/>
+      <c r="O18" s="10" t="n"/>
       <c r="P18" s="8" t="n"/>
       <c r="Q18" s="8" t="n"/>
       <c r="R18" s="8" t="n"/>
@@ -1690,7 +1690,7 @@
       <c r="Y18" s="8" t="n"/>
       <c r="Z18" s="8" t="n"/>
       <c r="AA18" s="8" t="n"/>
-      <c r="AB18" s="24" t="n"/>
+      <c r="AB18" s="5" t="n"/>
       <c r="AC18" s="8" t="n"/>
       <c r="AD18" s="15" t="n"/>
       <c r="AE18" s="8" t="n"/>
@@ -1771,20 +1771,20 @@
       <c r="T20" s="8" t="n"/>
       <c r="U20" s="8" t="n"/>
       <c r="V20" s="24" t="n"/>
-      <c r="W20" s="24" t="n"/>
+      <c r="W20" s="5" t="n"/>
       <c r="X20" s="8" t="n"/>
       <c r="Y20" s="8" t="n"/>
       <c r="Z20" s="8" t="n"/>
       <c r="AA20" s="8" t="n"/>
       <c r="AB20" s="8" t="n"/>
       <c r="AC20" s="24" t="n"/>
-      <c r="AD20" s="8" t="n"/>
+      <c r="AD20" s="24" t="n"/>
       <c r="AE20" s="8" t="n"/>
       <c r="AF20" s="8" t="n"/>
       <c r="AG20" s="8" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="27" t="inlineStr">
+      <c r="A21" s="26" t="inlineStr">
         <is>
           <t>9h</t>
         </is>
@@ -1794,40 +1794,40 @@
           <t>TPE</t>
         </is>
       </c>
-      <c r="C21" s="28" t="n"/>
-      <c r="D21" s="28" t="n"/>
-      <c r="E21" s="28" t="n"/>
-      <c r="F21" s="28" t="n"/>
-      <c r="G21" s="29" t="n"/>
-      <c r="H21" s="29" t="n"/>
-      <c r="I21" s="29" t="n"/>
-      <c r="J21" s="28" t="n"/>
-      <c r="K21" s="28" t="n"/>
-      <c r="L21" s="28" t="n"/>
-      <c r="M21" s="29" t="n"/>
-      <c r="N21" s="29" t="n"/>
-      <c r="O21" s="29" t="n"/>
-      <c r="P21" s="28" t="n"/>
-      <c r="Q21" s="28" t="n"/>
-      <c r="R21" s="28" t="n"/>
-      <c r="S21" s="28" t="n"/>
-      <c r="T21" s="28" t="n"/>
-      <c r="U21" s="29" t="n"/>
-      <c r="V21" s="29" t="n"/>
-      <c r="W21" s="29" t="n"/>
-      <c r="X21" s="28" t="n"/>
-      <c r="Y21" s="28" t="n"/>
-      <c r="Z21" s="28" t="n"/>
-      <c r="AA21" s="28" t="n"/>
-      <c r="AB21" s="29" t="n"/>
-      <c r="AC21" s="29" t="n"/>
-      <c r="AD21" s="29" t="n"/>
-      <c r="AE21" s="28" t="n"/>
-      <c r="AF21" s="28" t="n"/>
-      <c r="AG21" s="28" t="n"/>
+      <c r="C21" s="27" t="n"/>
+      <c r="D21" s="27" t="n"/>
+      <c r="E21" s="27" t="n"/>
+      <c r="F21" s="27" t="n"/>
+      <c r="G21" s="28" t="n"/>
+      <c r="H21" s="28" t="n"/>
+      <c r="I21" s="28" t="n"/>
+      <c r="J21" s="27" t="n"/>
+      <c r="K21" s="27" t="n"/>
+      <c r="L21" s="27" t="n"/>
+      <c r="M21" s="28" t="n"/>
+      <c r="N21" s="28" t="n"/>
+      <c r="O21" s="28" t="n"/>
+      <c r="P21" s="27" t="n"/>
+      <c r="Q21" s="27" t="n"/>
+      <c r="R21" s="27" t="n"/>
+      <c r="S21" s="27" t="n"/>
+      <c r="T21" s="27" t="n"/>
+      <c r="U21" s="28" t="n"/>
+      <c r="V21" s="28" t="n"/>
+      <c r="W21" s="28" t="n"/>
+      <c r="X21" s="27" t="n"/>
+      <c r="Y21" s="27" t="n"/>
+      <c r="Z21" s="27" t="n"/>
+      <c r="AA21" s="27" t="n"/>
+      <c r="AB21" s="28" t="n"/>
+      <c r="AC21" s="28" t="n"/>
+      <c r="AD21" s="28" t="n"/>
+      <c r="AE21" s="27" t="n"/>
+      <c r="AF21" s="27" t="n"/>
+      <c r="AG21" s="27" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="30" t="inlineStr">
+      <c r="A22" s="29" t="inlineStr">
         <is>
           <t>13h30</t>
         </is>
@@ -1843,34 +1843,34 @@
       <c r="F22" s="21" t="n"/>
       <c r="G22" s="21" t="n"/>
       <c r="H22" s="21" t="n"/>
-      <c r="I22" s="31" t="n"/>
+      <c r="I22" s="30" t="n"/>
       <c r="J22" s="21" t="n"/>
       <c r="K22" s="21" t="n"/>
       <c r="L22" s="21" t="n"/>
       <c r="M22" s="21" t="n"/>
       <c r="N22" s="21" t="n"/>
-      <c r="O22" s="31" t="n"/>
+      <c r="O22" s="30" t="n"/>
       <c r="P22" s="21" t="n"/>
-      <c r="Q22" s="31" t="n"/>
+      <c r="Q22" s="30" t="n"/>
       <c r="R22" s="21" t="n"/>
       <c r="S22" s="21" t="n"/>
       <c r="T22" s="21" t="n"/>
       <c r="U22" s="21" t="n"/>
       <c r="V22" s="21" t="n"/>
-      <c r="W22" s="31" t="n"/>
-      <c r="X22" s="31" t="n"/>
+      <c r="W22" s="30" t="n"/>
+      <c r="X22" s="30" t="n"/>
       <c r="Y22" s="21" t="n"/>
       <c r="Z22" s="21" t="n"/>
       <c r="AA22" s="21" t="n"/>
       <c r="AB22" s="21" t="n"/>
       <c r="AC22" s="21" t="n"/>
-      <c r="AD22" s="31" t="n"/>
-      <c r="AE22" s="31" t="n"/>
+      <c r="AD22" s="30" t="n"/>
+      <c r="AE22" s="30" t="n"/>
       <c r="AF22" s="21" t="n"/>
       <c r="AG22" s="21" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="32" t="inlineStr">
+      <c r="A23" s="31" t="inlineStr">
         <is>
           <t>13h30</t>
         </is>
@@ -1884,7 +1884,7 @@
       <c r="D23" s="8" t="n"/>
       <c r="E23" s="8" t="n"/>
       <c r="F23" s="8" t="n"/>
-      <c r="G23" s="5" t="n"/>
+      <c r="G23" s="8" t="n"/>
       <c r="H23" s="8" t="n"/>
       <c r="I23" s="8" t="n"/>
       <c r="J23" s="8" t="n"/>
@@ -1898,8 +1898,8 @@
       <c r="R23" s="8" t="n"/>
       <c r="S23" s="8" t="n"/>
       <c r="T23" s="8" t="n"/>
-      <c r="U23" s="25" t="n"/>
-      <c r="V23" s="8" t="n"/>
+      <c r="U23" s="8" t="n"/>
+      <c r="V23" s="25" t="n"/>
       <c r="W23" s="8" t="n"/>
       <c r="X23" s="8" t="n"/>
       <c r="Y23" s="8" t="n"/>
@@ -1913,7 +1913,7 @@
       <c r="AG23" s="8" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="32" t="inlineStr">
+      <c r="A24" s="31" t="inlineStr">
         <is>
           <t>13h30</t>
         </is>
@@ -1941,8 +1941,8 @@
       <c r="R24" s="8" t="n"/>
       <c r="S24" s="8" t="n"/>
       <c r="T24" s="8" t="n"/>
-      <c r="U24" s="8" t="n"/>
-      <c r="V24" s="25" t="n"/>
+      <c r="U24" s="25" t="n"/>
+      <c r="V24" s="8" t="n"/>
       <c r="W24" s="8" t="n"/>
       <c r="X24" s="8" t="n"/>
       <c r="Y24" s="8" t="n"/>
@@ -1956,7 +1956,7 @@
       <c r="AG24" s="8" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="32" t="inlineStr">
+      <c r="A25" s="31" t="inlineStr">
         <is>
           <t>13h30</t>
         </is>
@@ -1972,7 +1972,7 @@
       <c r="F25" s="8" t="n"/>
       <c r="G25" s="8" t="n"/>
       <c r="H25" s="8" t="n"/>
-      <c r="I25" s="25" t="n"/>
+      <c r="I25" s="8" t="n"/>
       <c r="J25" s="8" t="n"/>
       <c r="K25" s="8" t="n"/>
       <c r="L25" s="8" t="n"/>
@@ -1999,7 +1999,7 @@
       <c r="AG25" s="8" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="32" t="inlineStr">
+      <c r="A26" s="31" t="inlineStr">
         <is>
           <t>13h30</t>
         </is>
@@ -2015,7 +2015,7 @@
       <c r="F26" s="8" t="n"/>
       <c r="G26" s="8" t="n"/>
       <c r="H26" s="8" t="n"/>
-      <c r="I26" s="8" t="n"/>
+      <c r="I26" s="25" t="n"/>
       <c r="J26" s="8" t="n"/>
       <c r="K26" s="8" t="n"/>
       <c r="L26" s="8" t="n"/>
@@ -2042,7 +2042,7 @@
       <c r="AG26" s="8" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="32" t="inlineStr">
+      <c r="A27" s="31" t="inlineStr">
         <is>
           <t>13h30</t>
         </is>
@@ -2055,37 +2055,41 @@
       <c r="C27" s="8" t="n"/>
       <c r="D27" s="8" t="n"/>
       <c r="E27" s="8" t="n"/>
-      <c r="F27" s="15" t="n"/>
+      <c r="F27" s="5" t="n"/>
       <c r="G27" s="25" t="n"/>
-      <c r="H27" s="33" t="n"/>
+      <c r="H27" s="32" t="n"/>
       <c r="I27" s="24" t="n"/>
       <c r="J27" s="8" t="n"/>
       <c r="K27" s="8" t="n"/>
       <c r="L27" s="8" t="n"/>
       <c r="M27" s="24" t="n"/>
-      <c r="N27" s="34" t="n"/>
+      <c r="N27" s="5" t="n"/>
       <c r="O27" s="24" t="n"/>
       <c r="P27" s="8" t="n"/>
-      <c r="Q27" s="26" t="n"/>
+      <c r="Q27" s="10" t="n"/>
       <c r="R27" s="8" t="n"/>
       <c r="S27" s="8" t="n"/>
       <c r="T27" s="12" t="n"/>
-      <c r="U27" s="34" t="n"/>
+      <c r="U27" s="33" t="n"/>
       <c r="V27" s="15" t="n"/>
-      <c r="W27" s="33" t="n"/>
-      <c r="X27" s="10" t="n"/>
+      <c r="W27" s="32" t="n"/>
+      <c r="X27" s="34" t="inlineStr">
+        <is>
+          <t>V/C</t>
+        </is>
+      </c>
       <c r="Y27" s="8" t="n"/>
       <c r="Z27" s="8" t="n"/>
       <c r="AA27" s="8" t="n"/>
-      <c r="AB27" s="34" t="n"/>
+      <c r="AB27" s="33" t="n"/>
       <c r="AC27" s="24" t="n"/>
-      <c r="AD27" s="33" t="n"/>
+      <c r="AD27" s="32" t="n"/>
       <c r="AE27" s="24" t="n"/>
       <c r="AF27" s="8" t="n"/>
       <c r="AG27" s="8" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="32" t="inlineStr">
+      <c r="A28" s="31" t="inlineStr">
         <is>
           <t>13h30</t>
         </is>
@@ -2128,7 +2132,7 @@
       <c r="AG28" s="8" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="32" t="inlineStr">
+      <c r="A29" s="31" t="inlineStr">
         <is>
           <t>13h30</t>
         </is>
@@ -2171,7 +2175,7 @@
       <c r="AG29" s="8" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="32" t="inlineStr">
+      <c r="A30" s="31" t="inlineStr">
         <is>
           <t>13h30</t>
         </is>
@@ -2184,7 +2188,7 @@
       <c r="C30" s="8" t="n"/>
       <c r="D30" s="8" t="n"/>
       <c r="E30" s="8" t="n"/>
-      <c r="F30" s="26" t="n"/>
+      <c r="F30" s="10" t="n"/>
       <c r="G30" s="8" t="n"/>
       <c r="H30" s="10" t="n"/>
       <c r="I30" s="8" t="n"/>
@@ -2198,7 +2202,7 @@
       <c r="Q30" s="8" t="n"/>
       <c r="R30" s="8" t="n"/>
       <c r="S30" s="8" t="n"/>
-      <c r="T30" s="10" t="n"/>
+      <c r="T30" s="5" t="n"/>
       <c r="U30" s="8" t="n"/>
       <c r="V30" s="10" t="n"/>
       <c r="W30" s="8" t="n"/>
@@ -2214,7 +2218,7 @@
       <c r="AG30" s="8" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="32" t="inlineStr">
+      <c r="A31" s="31" t="inlineStr">
         <is>
           <t>13h30</t>
         </is>
@@ -2257,7 +2261,7 @@
       <c r="AG31" s="8" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="32" t="inlineStr">
+      <c r="A32" s="31" t="inlineStr">
         <is>
           <t>13h30</t>
         </is>
@@ -2270,7 +2274,7 @@
       <c r="C32" s="8" t="n"/>
       <c r="D32" s="8" t="n"/>
       <c r="E32" s="8" t="n"/>
-      <c r="F32" s="24" t="n"/>
+      <c r="F32" s="8" t="n"/>
       <c r="G32" s="8" t="n"/>
       <c r="H32" s="8" t="n"/>
       <c r="I32" s="8" t="n"/>
@@ -2284,7 +2288,7 @@
       <c r="Q32" s="8" t="n"/>
       <c r="R32" s="8" t="n"/>
       <c r="S32" s="8" t="n"/>
-      <c r="T32" s="24" t="n"/>
+      <c r="T32" s="5" t="n"/>
       <c r="U32" s="8" t="n"/>
       <c r="V32" s="8" t="n"/>
       <c r="W32" s="8" t="n"/>
@@ -2310,37 +2314,37 @@
           <t>TPE</t>
         </is>
       </c>
-      <c r="C33" s="28" t="n"/>
-      <c r="D33" s="28" t="n"/>
-      <c r="E33" s="28" t="n"/>
-      <c r="F33" s="28" t="n"/>
-      <c r="G33" s="29" t="n"/>
-      <c r="H33" s="29" t="n"/>
-      <c r="I33" s="29" t="n"/>
-      <c r="J33" s="28" t="n"/>
-      <c r="K33" s="28" t="n"/>
-      <c r="L33" s="28" t="n"/>
-      <c r="M33" s="29" t="n"/>
-      <c r="N33" s="29" t="n"/>
-      <c r="O33" s="29" t="n"/>
-      <c r="P33" s="28" t="n"/>
-      <c r="Q33" s="28" t="n"/>
-      <c r="R33" s="28" t="n"/>
-      <c r="S33" s="28" t="n"/>
-      <c r="T33" s="28" t="n"/>
-      <c r="U33" s="29" t="n"/>
-      <c r="V33" s="29" t="n"/>
-      <c r="W33" s="29" t="n"/>
-      <c r="X33" s="28" t="n"/>
-      <c r="Y33" s="28" t="n"/>
-      <c r="Z33" s="28" t="n"/>
-      <c r="AA33" s="28" t="n"/>
-      <c r="AB33" s="29" t="n"/>
-      <c r="AC33" s="29" t="n"/>
-      <c r="AD33" s="29" t="n"/>
-      <c r="AE33" s="28" t="n"/>
-      <c r="AF33" s="28" t="n"/>
-      <c r="AG33" s="28" t="n"/>
+      <c r="C33" s="27" t="n"/>
+      <c r="D33" s="27" t="n"/>
+      <c r="E33" s="27" t="n"/>
+      <c r="F33" s="27" t="n"/>
+      <c r="G33" s="28" t="n"/>
+      <c r="H33" s="28" t="n"/>
+      <c r="I33" s="28" t="n"/>
+      <c r="J33" s="27" t="n"/>
+      <c r="K33" s="27" t="n"/>
+      <c r="L33" s="27" t="n"/>
+      <c r="M33" s="28" t="n"/>
+      <c r="N33" s="28" t="n"/>
+      <c r="O33" s="28" t="n"/>
+      <c r="P33" s="27" t="n"/>
+      <c r="Q33" s="27" t="n"/>
+      <c r="R33" s="27" t="n"/>
+      <c r="S33" s="27" t="n"/>
+      <c r="T33" s="27" t="n"/>
+      <c r="U33" s="28" t="n"/>
+      <c r="V33" s="28" t="n"/>
+      <c r="W33" s="28" t="n"/>
+      <c r="X33" s="27" t="n"/>
+      <c r="Y33" s="27" t="n"/>
+      <c r="Z33" s="27" t="n"/>
+      <c r="AA33" s="27" t="n"/>
+      <c r="AB33" s="28" t="n"/>
+      <c r="AC33" s="28" t="n"/>
+      <c r="AD33" s="28" t="n"/>
+      <c r="AE33" s="27" t="n"/>
+      <c r="AF33" s="27" t="n"/>
+      <c r="AG33" s="27" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="36" t="inlineStr">
@@ -2396,37 +2400,37 @@
           <t>Aud. Civ.</t>
         </is>
       </c>
-      <c r="C35" s="28" t="n"/>
-      <c r="D35" s="28" t="n"/>
-      <c r="E35" s="28" t="n"/>
+      <c r="C35" s="27" t="n"/>
+      <c r="D35" s="27" t="n"/>
+      <c r="E35" s="27" t="n"/>
       <c r="F35" s="37" t="n"/>
-      <c r="G35" s="28" t="n"/>
+      <c r="G35" s="27" t="n"/>
       <c r="H35" s="37" t="n"/>
-      <c r="I35" s="28" t="n"/>
-      <c r="J35" s="28" t="n"/>
-      <c r="K35" s="28" t="n"/>
-      <c r="L35" s="28" t="n"/>
-      <c r="M35" s="28" t="n"/>
+      <c r="I35" s="27" t="n"/>
+      <c r="J35" s="27" t="n"/>
+      <c r="K35" s="27" t="n"/>
+      <c r="L35" s="27" t="n"/>
+      <c r="M35" s="27" t="n"/>
       <c r="N35" s="37" t="n"/>
-      <c r="O35" s="28" t="n"/>
-      <c r="P35" s="28" t="n"/>
-      <c r="Q35" s="28" t="n"/>
-      <c r="R35" s="28" t="n"/>
-      <c r="S35" s="28" t="n"/>
-      <c r="T35" s="28" t="n"/>
-      <c r="U35" s="28" t="n"/>
-      <c r="V35" s="28" t="n"/>
+      <c r="O35" s="27" t="n"/>
+      <c r="P35" s="27" t="n"/>
+      <c r="Q35" s="27" t="n"/>
+      <c r="R35" s="27" t="n"/>
+      <c r="S35" s="27" t="n"/>
+      <c r="T35" s="27" t="n"/>
+      <c r="U35" s="27" t="n"/>
+      <c r="V35" s="27" t="n"/>
       <c r="W35" s="37" t="n"/>
-      <c r="X35" s="28" t="n"/>
-      <c r="Y35" s="28" t="n"/>
-      <c r="Z35" s="28" t="n"/>
-      <c r="AA35" s="28" t="n"/>
-      <c r="AB35" s="28" t="n"/>
-      <c r="AC35" s="28" t="n"/>
-      <c r="AD35" s="28" t="n"/>
-      <c r="AE35" s="28" t="n"/>
-      <c r="AF35" s="28" t="n"/>
-      <c r="AG35" s="28" t="n"/>
+      <c r="X35" s="27" t="n"/>
+      <c r="Y35" s="27" t="n"/>
+      <c r="Z35" s="27" t="n"/>
+      <c r="AA35" s="27" t="n"/>
+      <c r="AB35" s="27" t="n"/>
+      <c r="AC35" s="27" t="n"/>
+      <c r="AD35" s="27" t="n"/>
+      <c r="AE35" s="27" t="n"/>
+      <c r="AF35" s="27" t="n"/>
+      <c r="AG35" s="27" t="n"/>
     </row>
     <row r="36">
       <c r="A36" s="38" t="inlineStr">
@@ -2488,7 +2492,7 @@
       <c r="F37" s="8" t="n"/>
       <c r="G37" s="8" t="n"/>
       <c r="H37" s="8" t="n"/>
-      <c r="I37" s="34" t="n"/>
+      <c r="I37" s="33" t="n"/>
       <c r="J37" s="8" t="n"/>
       <c r="K37" s="8" t="n"/>
       <c r="L37" s="8" t="n"/>
@@ -2502,14 +2506,14 @@
       <c r="T37" s="8" t="n"/>
       <c r="U37" s="8" t="n"/>
       <c r="V37" s="8" t="n"/>
-      <c r="W37" s="34" t="n"/>
+      <c r="W37" s="33" t="n"/>
       <c r="X37" s="8" t="n"/>
       <c r="Y37" s="8" t="n"/>
       <c r="Z37" s="8" t="n"/>
       <c r="AA37" s="8" t="n"/>
       <c r="AB37" s="8" t="n"/>
       <c r="AC37" s="8" t="n"/>
-      <c r="AD37" s="34" t="n"/>
+      <c r="AD37" s="33" t="n"/>
       <c r="AE37" s="8" t="n"/>
       <c r="AF37" s="8" t="n"/>
       <c r="AG37" s="8" t="n"/>
@@ -2528,30 +2532,30 @@
       <c r="C38" s="8" t="n"/>
       <c r="D38" s="8" t="n"/>
       <c r="E38" s="8" t="n"/>
-      <c r="F38" s="34" t="n"/>
+      <c r="F38" s="33" t="n"/>
       <c r="G38" s="8" t="n"/>
-      <c r="H38" s="34" t="n"/>
+      <c r="H38" s="33" t="n"/>
       <c r="I38" s="8" t="n"/>
       <c r="J38" s="8" t="n"/>
       <c r="K38" s="8" t="n"/>
       <c r="L38" s="8" t="n"/>
-      <c r="M38" s="34" t="n"/>
+      <c r="M38" s="33" t="n"/>
       <c r="N38" s="8" t="n"/>
-      <c r="O38" s="34" t="n"/>
+      <c r="O38" s="33" t="n"/>
       <c r="P38" s="8" t="n"/>
       <c r="Q38" s="8" t="n"/>
       <c r="R38" s="8" t="n"/>
       <c r="S38" s="8" t="n"/>
-      <c r="T38" s="34" t="n"/>
+      <c r="T38" s="33" t="n"/>
       <c r="U38" s="8" t="n"/>
-      <c r="V38" s="34" t="n"/>
+      <c r="V38" s="33" t="n"/>
       <c r="W38" s="8" t="n"/>
       <c r="X38" s="8" t="n"/>
       <c r="Y38" s="8" t="n"/>
       <c r="Z38" s="8" t="n"/>
       <c r="AA38" s="8" t="n"/>
       <c r="AB38" s="8" t="n"/>
-      <c r="AC38" s="34" t="n"/>
+      <c r="AC38" s="33" t="n"/>
       <c r="AD38" s="8" t="n"/>
       <c r="AE38" s="8" t="n"/>
       <c r="AF38" s="8" t="n"/>
@@ -2574,7 +2578,7 @@
       <c r="F39" s="8" t="n"/>
       <c r="G39" s="8" t="n"/>
       <c r="H39" s="8" t="n"/>
-      <c r="I39" s="34" t="n"/>
+      <c r="I39" s="33" t="n"/>
       <c r="J39" s="8" t="n"/>
       <c r="K39" s="8" t="n"/>
       <c r="L39" s="8" t="n"/>
@@ -2588,14 +2592,14 @@
       <c r="T39" s="8" t="n"/>
       <c r="U39" s="8" t="n"/>
       <c r="V39" s="8" t="n"/>
-      <c r="W39" s="34" t="n"/>
+      <c r="W39" s="33" t="n"/>
       <c r="X39" s="8" t="n"/>
       <c r="Y39" s="8" t="n"/>
       <c r="Z39" s="8" t="n"/>
       <c r="AA39" s="8" t="n"/>
       <c r="AB39" s="8" t="n"/>
       <c r="AC39" s="8" t="n"/>
-      <c r="AD39" s="34" t="n"/>
+      <c r="AD39" s="33" t="n"/>
       <c r="AE39" s="8" t="n"/>
       <c r="AF39" s="8" t="n"/>
       <c r="AG39" s="8" t="n"/>
@@ -2611,37 +2615,37 @@
           <t>CJ</t>
         </is>
       </c>
-      <c r="C40" s="28" t="n"/>
-      <c r="D40" s="28" t="n"/>
-      <c r="E40" s="28" t="n"/>
-      <c r="F40" s="28" t="n"/>
-      <c r="G40" s="28" t="n"/>
-      <c r="H40" s="28" t="n"/>
-      <c r="I40" s="28" t="n"/>
-      <c r="J40" s="28" t="n"/>
-      <c r="K40" s="28" t="n"/>
-      <c r="L40" s="28" t="n"/>
-      <c r="M40" s="28" t="n"/>
-      <c r="N40" s="28" t="n"/>
-      <c r="O40" s="28" t="n"/>
-      <c r="P40" s="28" t="n"/>
-      <c r="Q40" s="28" t="n"/>
-      <c r="R40" s="28" t="n"/>
-      <c r="S40" s="28" t="n"/>
-      <c r="T40" s="28" t="n"/>
-      <c r="U40" s="28" t="n"/>
-      <c r="V40" s="28" t="n"/>
-      <c r="W40" s="28" t="n"/>
-      <c r="X40" s="28" t="n"/>
-      <c r="Y40" s="28" t="n"/>
-      <c r="Z40" s="28" t="n"/>
-      <c r="AA40" s="28" t="n"/>
-      <c r="AB40" s="28" t="n"/>
-      <c r="AC40" s="28" t="n"/>
-      <c r="AD40" s="28" t="n"/>
-      <c r="AE40" s="28" t="n"/>
-      <c r="AF40" s="28" t="n"/>
-      <c r="AG40" s="28" t="n"/>
+      <c r="C40" s="27" t="n"/>
+      <c r="D40" s="27" t="n"/>
+      <c r="E40" s="27" t="n"/>
+      <c r="F40" s="27" t="n"/>
+      <c r="G40" s="27" t="n"/>
+      <c r="H40" s="27" t="n"/>
+      <c r="I40" s="27" t="n"/>
+      <c r="J40" s="27" t="n"/>
+      <c r="K40" s="27" t="n"/>
+      <c r="L40" s="27" t="n"/>
+      <c r="M40" s="27" t="n"/>
+      <c r="N40" s="27" t="n"/>
+      <c r="O40" s="27" t="n"/>
+      <c r="P40" s="27" t="n"/>
+      <c r="Q40" s="27" t="n"/>
+      <c r="R40" s="27" t="n"/>
+      <c r="S40" s="27" t="n"/>
+      <c r="T40" s="27" t="n"/>
+      <c r="U40" s="27" t="n"/>
+      <c r="V40" s="27" t="n"/>
+      <c r="W40" s="27" t="n"/>
+      <c r="X40" s="27" t="n"/>
+      <c r="Y40" s="27" t="n"/>
+      <c r="Z40" s="27" t="n"/>
+      <c r="AA40" s="27" t="n"/>
+      <c r="AB40" s="27" t="n"/>
+      <c r="AC40" s="27" t="n"/>
+      <c r="AD40" s="27" t="n"/>
+      <c r="AE40" s="27" t="n"/>
+      <c r="AF40" s="27" t="n"/>
+      <c r="AG40" s="27" t="n"/>
     </row>
     <row r="41">
       <c r="A41" s="42" t="inlineStr">
@@ -2701,28 +2705,28 @@
       <c r="D42" s="8" t="n"/>
       <c r="E42" s="8" t="n"/>
       <c r="F42" s="8" t="n"/>
-      <c r="G42" s="25" t="n"/>
+      <c r="G42" s="5" t="n"/>
       <c r="H42" s="25" t="n"/>
       <c r="I42" s="25" t="n"/>
       <c r="J42" s="8" t="n"/>
       <c r="K42" s="8" t="n"/>
       <c r="L42" s="8" t="n"/>
       <c r="M42" s="8" t="n"/>
-      <c r="N42" s="25" t="n"/>
+      <c r="N42" s="5" t="n"/>
       <c r="O42" s="25" t="n"/>
       <c r="P42" s="8" t="n"/>
       <c r="Q42" s="8" t="n"/>
       <c r="R42" s="8" t="n"/>
       <c r="S42" s="8" t="n"/>
       <c r="T42" s="8" t="n"/>
-      <c r="U42" s="25" t="n"/>
+      <c r="U42" s="5" t="n"/>
       <c r="V42" s="25" t="n"/>
       <c r="W42" s="25" t="n"/>
       <c r="X42" s="8" t="n"/>
       <c r="Y42" s="8" t="n"/>
       <c r="Z42" s="8" t="n"/>
       <c r="AA42" s="8" t="n"/>
-      <c r="AB42" s="25" t="n"/>
+      <c r="AB42" s="5" t="n"/>
       <c r="AC42" s="25" t="n"/>
       <c r="AD42" s="25" t="n"/>
       <c r="AE42" s="8" t="n"/>
@@ -2740,37 +2744,37 @@
           <t>T Com</t>
         </is>
       </c>
-      <c r="C43" s="28" t="n"/>
-      <c r="D43" s="28" t="n"/>
-      <c r="E43" s="28" t="n"/>
-      <c r="F43" s="28" t="n"/>
+      <c r="C43" s="27" t="n"/>
+      <c r="D43" s="27" t="n"/>
+      <c r="E43" s="27" t="n"/>
+      <c r="F43" s="27" t="n"/>
       <c r="G43" s="46" t="n"/>
-      <c r="H43" s="28" t="n"/>
-      <c r="I43" s="28" t="n"/>
-      <c r="J43" s="28" t="n"/>
-      <c r="K43" s="28" t="n"/>
-      <c r="L43" s="28" t="n"/>
-      <c r="M43" s="28" t="n"/>
-      <c r="N43" s="28" t="n"/>
-      <c r="O43" s="28" t="n"/>
-      <c r="P43" s="28" t="n"/>
-      <c r="Q43" s="28" t="n"/>
-      <c r="R43" s="28" t="n"/>
-      <c r="S43" s="28" t="n"/>
-      <c r="T43" s="28" t="n"/>
-      <c r="U43" s="28" t="n"/>
-      <c r="V43" s="28" t="n"/>
+      <c r="H43" s="27" t="n"/>
+      <c r="I43" s="27" t="n"/>
+      <c r="J43" s="27" t="n"/>
+      <c r="K43" s="27" t="n"/>
+      <c r="L43" s="27" t="n"/>
+      <c r="M43" s="27" t="n"/>
+      <c r="N43" s="27" t="n"/>
+      <c r="O43" s="27" t="n"/>
+      <c r="P43" s="27" t="n"/>
+      <c r="Q43" s="27" t="n"/>
+      <c r="R43" s="27" t="n"/>
+      <c r="S43" s="27" t="n"/>
+      <c r="T43" s="27" t="n"/>
+      <c r="U43" s="27" t="n"/>
+      <c r="V43" s="27" t="n"/>
       <c r="W43" s="46" t="n"/>
-      <c r="X43" s="28" t="n"/>
-      <c r="Y43" s="28" t="n"/>
-      <c r="Z43" s="28" t="n"/>
-      <c r="AA43" s="28" t="n"/>
-      <c r="AB43" s="28" t="n"/>
-      <c r="AC43" s="28" t="n"/>
-      <c r="AD43" s="28" t="n"/>
-      <c r="AE43" s="28" t="n"/>
-      <c r="AF43" s="28" t="n"/>
-      <c r="AG43" s="28" t="n"/>
+      <c r="X43" s="27" t="n"/>
+      <c r="Y43" s="27" t="n"/>
+      <c r="Z43" s="27" t="n"/>
+      <c r="AA43" s="27" t="n"/>
+      <c r="AB43" s="27" t="n"/>
+      <c r="AC43" s="27" t="n"/>
+      <c r="AD43" s="27" t="n"/>
+      <c r="AE43" s="27" t="n"/>
+      <c r="AF43" s="27" t="n"/>
+      <c r="AG43" s="27" t="n"/>
     </row>
     <row r="44">
       <c r="A44" s="47" t="inlineStr">

</xml_diff>